<commit_message>
Adding 2020 reader analysis
</commit_message>
<xml_diff>
--- a/dataset/2020_pythonmarketer.com_post_views.xlsx
+++ b/dataset/2020_pythonmarketer.com_post_views.xlsx
@@ -77,7 +77,7 @@
   <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -89,12 +89,12 @@
     <row r="1" spans="1:2">
       <c r="A1" t="inlineStr">
         <is>
-          <t>blog_post_name</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>views</t>
+          <t>Views</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added post urls to 2020 post data
</commit_message>
<xml_diff>
--- a/dataset/2020_pythonmarketer.com_post_views.xlsx
+++ b/dataset/2020_pythonmarketer.com_post_views.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="19200" windowHeight="7830"/>
+    <workbookView activeTab="0" windowWidth="17080" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="pythonmarketer.com_posts_year_01_01_2020_12_31_2020.csv" sheetId="1" r:id="rId1"/>
@@ -74,31 +74,38 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" style="0" width="91.13737980769231" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" style="0" width="9.142307692307693"/>
+    <col min="2" max="2" style="0" width="9.142307692307693"/>
+    <col min="3" max="3" style="0" width="144.84843750000002" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Views</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+          <t>views</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="inlineStr">
         <is>
           <t>Home page / Archives</t>
@@ -107,8 +114,13 @@
       <c r="B2">
         <v>1013</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="inlineStr">
         <is>
           <t>Gooey GUI for Python Scripts</t>
@@ -117,8 +129,13 @@
       <c r="B3">
         <v>610</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2018/08/25/gooey-gui-for-python-scripts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="inlineStr">
         <is>
           <t>Inserting New Rows Into A Microsoft Access Database With Python and pyodbc</t>
@@ -127,8 +144,13 @@
       <c r="B4">
         <v>594</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2019/11/30/inserting-new-records-into-a-microsoft-access-database-with-python/</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="inlineStr">
         <is>
           <t>How to Install Libraries and Enable the pip Installer in Python</t>
@@ -137,8 +159,13 @@
       <c r="B5">
         <v>579</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2018/01/20/how-to-python-pip-install-new-libraries/</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="inlineStr">
         <is>
           <t>Making A Desktop Color Eyedropper in Python to Grab Color Values</t>
@@ -147,8 +174,13 @@
       <c r="B6">
         <v>226</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2018/09/14/making-a-python-eyedropper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="inlineStr">
         <is>
           <t>Integrating MySQL with Flask, pandas and pythonanywhere</t>
@@ -157,8 +189,13 @@
       <c r="B7">
         <v>221</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/05/25/essential-mysql-terminal-commands-and-connecting-to-mysql-with-flask-pandas-and-pythonanywhere/</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="inlineStr">
         <is>
           <t>Findstr, RegEx File Searches for Windows</t>
@@ -167,8 +204,13 @@
       <c r="B8">
         <v>184</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2018/07/15/findstr-aka-grep-for-windows/</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="inlineStr">
         <is>
           <t>Automating pytest on Windows with a .bat file, Python, Task Scheduler and Box</t>
@@ -177,8 +219,13 @@
       <c r="B9">
         <v>133</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/03/21/automating-pytest-on-windows-with-a-bat-file-python-task-scheduler-and-box/</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="inlineStr">
         <is>
           <t>Packaging Python as a Windows App via Pyinstaller</t>
@@ -187,8 +234,13 @@
       <c r="B10">
         <v>101</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2018/11/20/packaging-python-as-a-windows-app/</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="inlineStr">
         <is>
           <t>Delete All Your Tweets with Tweepy and the Twitter API</t>
@@ -197,8 +249,13 @@
       <c r="B11">
         <v>97</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/09/13/delete-all-your-tweets-with-tweepy-and-the-twitter-api/</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="inlineStr">
         <is>
           <t>A Guide To Making HTTP Requests To APIs With JSON &amp; Python</t>
@@ -207,8 +264,13 @@
       <c r="B12">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/05/18/how-to-make-json-requests-with-python/</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="inlineStr">
         <is>
           <t>Automated Python With Windows Task Scheduler</t>
@@ -217,8 +279,13 @@
       <c r="B13">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2018/11/25/automated-python-with-windows-task-scheduler/</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="inlineStr">
         <is>
           <t>Comparing Text Editors on Ubuntu: Atom, Emacs, Sublime, Vim &amp; VS Code</t>
@@ -227,8 +294,13 @@
       <c r="B14">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2019/12/26/comparing-text-editors-on-ubuntu-atom-emacs-sublime-vim-vs-code/</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="inlineStr">
         <is>
           <t>Plotting Datasets Using Jupyter, Pandas and Matplotlib</t>
@@ -237,8 +309,13 @@
       <c r="B15">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2019/04/12/datasets-plotting-using-jupyter-pandas-and-matplotlib/</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="inlineStr">
         <is>
           <t>Copying a pandas Dataframe to Google Sheets with pygsheets</t>
@@ -247,8 +324,13 @@
       <c r="B16">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2019/12/21/copying-a-csv-file-to-google-sheets-with-pygsheets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="inlineStr">
         <is>
           <t>Making A YouTube Video Downloader With Python's Flask and pytube3 Libraries</t>
@@ -257,8 +339,13 @@
       <c r="B17">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/10/07/making-a-youtube-video-downloader-with-pythons-flask-and-pytube3-libraries/</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="inlineStr">
         <is>
           <t>Benefits of Go and Threads in Distributed Systems</t>
@@ -267,8 +354,13 @@
       <c r="B18">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/07/15/benefits-of-go-and-threads-in-distributed-systems/</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="inlineStr">
         <is>
           <t>A Stroll Through Pandas 1.0, Python’s Tabular Data Powerhouse</t>
@@ -277,8 +369,13 @@
       <c r="B19">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2018/05/12/pandas-pythons-excel-powerhouse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="inlineStr">
         <is>
           <t>Google Vision OCR, Image Text and a Markov Chain: a recipe for positivipy</t>
@@ -287,8 +384,13 @@
       <c r="B20">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/10/11/generating-positive-thoughts-with-google-vision-ocr-and-markov-chains/</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="inlineStr">
         <is>
           <t>Script Windows Like A Pro: Command Line, Batch Files, Remote Desktop Connection and pywin32</t>
@@ -297,8 +399,13 @@
       <c r="B21">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/05/06/exploring-windows-command-line-tools-batch-file-automation-and-remote-desktop-connection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="inlineStr">
         <is>
           <t>WTF is a Regression</t>
@@ -307,8 +414,13 @@
       <c r="B22">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2018/10/19/wtf-is-a-regression/</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="inlineStr">
         <is>
           <t>Free Computer Science Courses and Talks To Absorb</t>
@@ -317,8 +429,13 @@
       <c r="B23">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/06/23/my-favorite-free-educational-courses-and-talks-to-absorb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="inlineStr">
         <is>
           <t>Installing Debian 9 Stretch Linux OS on a Dell Inspiron Laptop and Configuring the Wifi Network</t>
@@ -327,8 +444,13 @@
       <c r="B24">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2019/04/25/installing-debian-9-stretch-linux-os-on-a-dell-inspiron-laptop-and-troubleshooting-wifi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="inlineStr">
         <is>
           <t>Reflections on 5 Years of Solving Problems with Python</t>
@@ -337,8 +459,13 @@
       <c r="B25">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/04/11/reflections-on-5-years-of-solving-problems-with-python/</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="inlineStr">
         <is>
           <t>Lessons Learned from "Lost in Space</t>
@@ -347,8 +474,13 @@
       <c r="B26">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/01/28/lessons-learned-from-lost-in-space-on-netflix/</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="inlineStr">
         <is>
           <t>SQLite3: Pythonic First Impressions &amp; Lay of the Land</t>
@@ -357,8 +489,13 @@
       <c r="B27">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/09/20/getting-the-lay-of-the-land-in-sqlite-and-connecting-to-a-db-with-pythons-sqlite3-library/</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="inlineStr">
         <is>
           <t>Tkinter and Python Libraries</t>
@@ -367,8 +504,13 @@
       <c r="B28">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2016/02/29/tkinter-and-python-libraries/</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="inlineStr">
         <is>
           <t>Creating Isolated Python Environments with Virtualenv</t>
@@ -377,8 +519,13 @@
       <c r="B29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2018/04/10/creating-isolated-python-environments-with-virtualenv/</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="inlineStr">
         <is>
           <t>Getting Started With web2py</t>
@@ -387,8 +534,13 @@
       <c r="B30">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2016/03/29/getting-started-with-web2py/</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="inlineStr">
         <is>
           <t>Characterizing Database Workloads &amp; Storage Models</t>
@@ -397,8 +549,13 @@
       <c r="B31">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/06/27/choosing-database-storage-models-and-workloads-that-mesh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="inlineStr">
         <is>
           <t>A Collection of Software Testing Opinions for Python and Beyond</t>
@@ -407,8 +564,13 @@
       <c r="B32">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2019/12/05/a-collection-of-software-testing-opinions-for-python-and-beyond/</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="inlineStr">
         <is>
           <t>Post an Unsplash Photo to Facebook Pages with Python</t>
@@ -417,8 +579,13 @@
       <c r="B33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/10/04/post-a-photo-to-your-facebook-page-with-the-unsplash-facebook-apis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="inlineStr">
         <is>
           <t>Lightning Scripts ⚡</t>
@@ -427,8 +594,13 @@
       <c r="B34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2019/02/12/lightning-scripts-%e2%9a%a1/</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="inlineStr">
         <is>
           <t>Scripting As Simplified Cognition (How to Catch A Flight)</t>
@@ -437,8 +609,13 @@
       <c r="B35">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/07/22/the-beauty-of-scripting-write-scripts-and-follow-them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="inlineStr">
         <is>
           <t>Cleaning Data with Python and Excel: A Brief Example</t>
@@ -447,8 +624,13 @@
       <c r="B36">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2018/03/30/cleaning-data-with-python/</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="inlineStr">
         <is>
           <t>Ask Tame Impala - My First Web App</t>
@@ -457,8 +639,13 @@
       <c r="B37">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2016/05/25/askkevinparker-com-my-first-web-app-other-notes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="inlineStr">
         <is>
           <t>Maximize Your Energy Through Trade-offs and Specialization in Life Choices</t>
@@ -467,8 +654,13 @@
       <c r="B38">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/09/12/leveraging-specialization-and-considering-trade-offs-in-decision-making/</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="inlineStr">
         <is>
           <t>Useful Links for web2py Beginners</t>
@@ -477,8 +669,13 @@
       <c r="B39">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2016/04/30/useful-links-for-web2py-beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="inlineStr">
         <is>
           <t>Creating A Simple Website and Server Environment with Node.js and Express.js</t>
@@ -487,8 +684,13 @@
       <c r="B40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2017/08/09/creating-a-simple-website-and-server-environment-with-node-js-and-express-js/</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="inlineStr">
         <is>
           <t>The Joy of Logging With Python</t>
@@ -497,8 +699,13 @@
       <c r="B41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2019/02/02/the-joy-of-logging-with-python/</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" t="inlineStr">
         <is>
           <t>Choosing a Web Development Path</t>
@@ -507,8 +714,13 @@
       <c r="B42">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2016/03/22/choosing-a-web-development-path/</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="inlineStr">
         <is>
           <t>Pondering Join Algorithms</t>
@@ -517,8 +729,13 @@
       <c r="B43">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/08/09/join-algorithms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="inlineStr">
         <is>
           <t>Oversimplified Javascript Terms</t>
@@ -527,8 +744,13 @@
       <c r="B44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2017/08/05/oversimplified-javascript-terms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="inlineStr">
         <is>
           <t>Discoveries['Random']</t>
@@ -537,8 +759,13 @@
       <c r="B45">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2016/03/11/random-findings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" t="inlineStr">
         <is>
           <t>Python Koans</t>
@@ -547,8 +774,13 @@
       <c r="B46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2016/02/23/dotd-python-koans/</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" t="inlineStr">
         <is>
           <t>20 Eclectic Computer Science Wikipedia Articles</t>
@@ -557,8 +789,13 @@
       <c r="B47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/11/28/a-computer-science-themed-wikipedia-link-grab-bag/</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" t="inlineStr">
         <is>
           <t>Reasons to Explore Rust and A Brief Intro</t>
@@ -567,8 +804,13 @@
       <c r="B48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2019/08/19/choosing-rust-as-my-second-language/</t>
+        </is>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="inlineStr">
         <is>
           <t>On Learning New Things</t>
@@ -577,8 +819,13 @@
       <c r="B49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2016/04/05/on-learning-new-things/</t>
+        </is>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="inlineStr">
         <is>
           <t>Easy Tune-ups For Your Windows Computer</t>
@@ -587,8 +834,13 @@
       <c r="B50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/03/22/easy-wins-for-your-windows-computer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="inlineStr">
         <is>
           <t>Assessing The Marketing Effects of Randomization Failure</t>
@@ -597,18 +849,28 @@
       <c r="B51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/05/09/when-random-isnt-so-random-the-time-i-accidentally-postcard-bombed-some-people/</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="inlineStr">
         <is>
-          <t>"Git the Basics" A Version Control Cheat Sheet</t>
+          <t>"Git" the Basics: A Version Control Cheat Sheet</t>
         </is>
       </c>
       <c r="B52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2020/01/25/git-the-basics-a-git-version-control-cheat-sheet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" t="inlineStr">
         <is>
           <t>Python File Handling Basics</t>
@@ -617,8 +879,13 @@
       <c r="B53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2018/01/14/python-file-handling-basics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="inlineStr">
         <is>
           <t>Algorithms Will Decide The Future</t>
@@ -627,8 +894,13 @@
       <c r="B54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2017/08/01/algorithms-will-decide-the-future/</t>
+        </is>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="inlineStr">
         <is>
           <t>Tips For Creating Useful Ideas</t>
@@ -637,8 +909,13 @@
       <c r="B55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2017/07/30/how-to-create-things-people-care-about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" t="inlineStr">
         <is>
           <t>Marketer Slash Programmer</t>
@@ -646,6 +923,11 @@
       </c>
       <c r="B56">
         <v>1</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>https://pythonmarketer.wordpress.com/2016/02/22/marketer-slash-programmer/</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>